<commit_message>
Docs:changes to data repo from updated functions
</commit_message>
<xml_diff>
--- a/encoded_data_final.xlsx
+++ b/encoded_data_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS99"/>
+  <dimension ref="A1:AI99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,117 +546,67 @@
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR ANNUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
+          <t>Recommended Action_Cleaned_FOR ANNUAL FOLLOW-UP AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR ANUAL FOLLOW UP AND PAP SMEAR IN 3 YEARS</t>
+          <t>Recommended Action_Cleaned_FOR BIOPSY AND CYTOLOGY (TAH NOT RECOMMENDED)</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR BIOPSY AND CYTOLOGY WITH TAH NOT RECOMMENDED</t>
+          <t>Recommended Action_Cleaned_FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR COLOSCOPY BIOSY, CYTOLOGY</t>
+          <t>Recommended Action_Cleaned_FOR COLPOSCOPY, BIOPSY, AND CYTOLOGY (TAH NOT RECOMMENDED)</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR COLPOSCOPY BIOPSY AND CYTOLOGY+/- TAH</t>
+          <t>Recommended Action_Cleaned_FOR COLPOSCOPY, BIOPSY, CYTOLOGY +/- TAH</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR COLPOSCOPY BIOPSY, CYTOLOGY</t>
+          <t>Recommended Action_Cleaned_FOR COLPOSCOPY, CYTOLOGY, THEN LASER THERAPY</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR COLPOSCOPY BIOPSY, CYTOLOGY +/-TAH</t>
+          <t>Recommended Action_Cleaned_FOR HPV VACCINE AND SEXUAL EDUCATION</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR COLPOSCOPY BIOSPY, CYTOLOGY</t>
+          <t>Recommended Action_Cleaned_FOR HPV VACCINE, LIFESTYLE, AND SEXUAL EDUCATION</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR COLPOSCOPY BIOSPY, CYTOLOGY +/- TAH</t>
+          <t>Recommended Action_Cleaned_FOR LASER THERAPY</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR COLPOSCOPY BIOSY, CYTOLOGY+/- TAH</t>
+          <t>Recommended Action_Cleaned_FOR PAP SMEAR</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR COLPOSCOPY CYTOLOGY AND BIOPSY</t>
+          <t>Recommended Action_Cleaned_FOR REPEAT HPV TESTING ANNUALLY AND PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR COLPOSCPY BIOPSY, CYTOLOGY</t>
+          <t>Recommended Action_Cleaned_REPEAT PAP SMEAR IN 3 YEARS</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>Recommended Action_FOR COLPOSOCPY BIOPSY, CYTOLOGY WITH TAH NOT RECOMMENDED</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_FOR HPV VACCINATION AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_FOR HPV VACCINE AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_FOR HPV VACCINE, LIFESTYLE AND SEXUAL EDUCATION</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_FOR LASER THERAPY</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_FOR PAP SMEAR</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_FOR REPEAT HPV TESTING ANNUALLY AND PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_FORCOLPOSCOPY, CYTOLOGY THEN LASER THERAPY</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_REPEAT PAP SMEAR IN 3 YEARS</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_REPEAT PAP SMEAR IN 3 YEARS AND FOR HPV VACCINE</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>Recommended Action_REPEAT PAP SMEAR IN 3YEARS</t>
+          <t>Recommended Action_Cleaned_REPEAT PAP SMEAR IN 3 YEARS AND FOR HPV VACCINE</t>
         </is>
       </c>
     </row>
@@ -764,37 +714,7 @@
         <v>0</v>
       </c>
       <c r="AI2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -883,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="AC3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -901,36 +821,6 @@
         <v>0</v>
       </c>
       <c r="AI3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1020,7 +910,7 @@
         <v>0</v>
       </c>
       <c r="AC4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -1038,36 +928,6 @@
         <v>0</v>
       </c>
       <c r="AI4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1160,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="AD5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE5" t="n">
         <v>0</v>
@@ -1175,36 +1035,6 @@
         <v>0</v>
       </c>
       <c r="AI5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1294,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="AC6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
@@ -1312,36 +1142,6 @@
         <v>0</v>
       </c>
       <c r="AI6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1449,37 +1249,7 @@
         <v>0</v>
       </c>
       <c r="AI7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -1556,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8" t="n">
         <v>0</v>
@@ -1580,42 +1350,12 @@
         <v>0</v>
       </c>
       <c r="AG8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH8" t="n">
         <v>0</v>
       </c>
       <c r="AI8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1720,39 +1460,9 @@
         <v>0</v>
       </c>
       <c r="AH9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1836,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="AA10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10" t="n">
         <v>0</v>
@@ -1851,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="AF10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG10" t="n">
         <v>0</v>
@@ -1860,36 +1570,6 @@
         <v>0</v>
       </c>
       <c r="AI10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1964,10 +1644,10 @@
         <v>0</v>
       </c>
       <c r="X11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z11" t="n">
         <v>0</v>
@@ -1997,36 +1677,6 @@
         <v>0</v>
       </c>
       <c r="AI11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2131,39 +1781,9 @@
         <v>0</v>
       </c>
       <c r="AH12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2268,39 +1888,9 @@
         <v>0</v>
       </c>
       <c r="AH13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2378,7 +1968,7 @@
         <v>0</v>
       </c>
       <c r="Y14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z14" t="n">
         <v>0</v>
@@ -2387,7 +1977,7 @@
         <v>0</v>
       </c>
       <c r="AB14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC14" t="n">
         <v>0</v>
@@ -2408,36 +1998,6 @@
         <v>0</v>
       </c>
       <c r="AI14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2515,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="Y15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z15" t="n">
         <v>0</v>
@@ -2524,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="AB15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC15" t="n">
         <v>0</v>
@@ -2545,36 +2105,6 @@
         <v>0</v>
       </c>
       <c r="AI15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2684,36 +2214,6 @@
       <c r="AI16" t="n">
         <v>0</v>
       </c>
-      <c r="AJ16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS16" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2789,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="Y17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z17" t="n">
         <v>0</v>
@@ -2798,7 +2298,7 @@
         <v>0</v>
       </c>
       <c r="AB17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC17" t="n">
         <v>0</v>
@@ -2819,36 +2319,6 @@
         <v>0</v>
       </c>
       <c r="AI17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2953,39 +2423,9 @@
         <v>0</v>
       </c>
       <c r="AH18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3090,39 +2530,9 @@
         <v>0</v>
       </c>
       <c r="AH19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3227,39 +2637,9 @@
         <v>0</v>
       </c>
       <c r="AH20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3369,36 +2749,6 @@
       <c r="AI21" t="n">
         <v>0</v>
       </c>
-      <c r="AJ21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS21" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -3501,39 +2851,9 @@
         <v>0</v>
       </c>
       <c r="AH22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ22" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3638,39 +2958,9 @@
         <v>0</v>
       </c>
       <c r="AH23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ23" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3775,39 +3065,9 @@
         <v>0</v>
       </c>
       <c r="AH24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ24" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3897,7 +3157,7 @@
         <v>0</v>
       </c>
       <c r="AC25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD25" t="n">
         <v>0</v>
@@ -3915,36 +3175,6 @@
         <v>0</v>
       </c>
       <c r="AI25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK25" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4022,7 +3252,7 @@
         <v>0</v>
       </c>
       <c r="Y26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z26" t="n">
         <v>0</v>
@@ -4031,7 +3261,7 @@
         <v>0</v>
       </c>
       <c r="AB26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC26" t="n">
         <v>0</v>
@@ -4052,36 +3282,6 @@
         <v>0</v>
       </c>
       <c r="AI26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4159,7 +3359,7 @@
         <v>0</v>
       </c>
       <c r="Y27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z27" t="n">
         <v>0</v>
@@ -4168,7 +3368,7 @@
         <v>0</v>
       </c>
       <c r="AB27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC27" t="n">
         <v>0</v>
@@ -4189,36 +3389,6 @@
         <v>0</v>
       </c>
       <c r="AI27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4296,7 +3466,7 @@
         <v>0</v>
       </c>
       <c r="Y28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z28" t="n">
         <v>0</v>
@@ -4305,7 +3475,7 @@
         <v>0</v>
       </c>
       <c r="AB28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC28" t="n">
         <v>0</v>
@@ -4326,36 +3496,6 @@
         <v>0</v>
       </c>
       <c r="AI28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4465,36 +3605,6 @@
       <c r="AI29" t="n">
         <v>0</v>
       </c>
-      <c r="AJ29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS29" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -4597,39 +3707,9 @@
         <v>0</v>
       </c>
       <c r="AH30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ30" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4728,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="AF31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG31" t="n">
         <v>0</v>
@@ -4737,36 +3817,6 @@
         <v>0</v>
       </c>
       <c r="AI31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN31" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4876,36 +3926,6 @@
       <c r="AI32" t="n">
         <v>0</v>
       </c>
-      <c r="AJ32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS32" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -5002,7 +4022,7 @@
         <v>0</v>
       </c>
       <c r="AF33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG33" t="n">
         <v>0</v>
@@ -5011,36 +4031,6 @@
         <v>0</v>
       </c>
       <c r="AI33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN33" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5150,36 +4140,6 @@
       <c r="AI34" t="n">
         <v>0</v>
       </c>
-      <c r="AJ34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS34" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -5255,7 +4215,7 @@
         <v>0</v>
       </c>
       <c r="Y35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z35" t="n">
         <v>0</v>
@@ -5264,7 +4224,7 @@
         <v>0</v>
       </c>
       <c r="AB35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC35" t="n">
         <v>0</v>
@@ -5285,36 +4245,6 @@
         <v>0</v>
       </c>
       <c r="AI35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5392,7 +4322,7 @@
         <v>0</v>
       </c>
       <c r="Y36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z36" t="n">
         <v>0</v>
@@ -5401,7 +4331,7 @@
         <v>0</v>
       </c>
       <c r="AB36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC36" t="n">
         <v>0</v>
@@ -5422,36 +4352,6 @@
         <v>0</v>
       </c>
       <c r="AI36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5550,7 +4450,7 @@
         <v>0</v>
       </c>
       <c r="AF37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG37" t="n">
         <v>0</v>
@@ -5559,36 +4459,6 @@
         <v>0</v>
       </c>
       <c r="AI37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN37" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5666,7 +4536,7 @@
         <v>0</v>
       </c>
       <c r="Y38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z38" t="n">
         <v>0</v>
@@ -5675,7 +4545,7 @@
         <v>0</v>
       </c>
       <c r="AB38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC38" t="n">
         <v>0</v>
@@ -5696,36 +4566,6 @@
         <v>0</v>
       </c>
       <c r="AI38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5824,7 +4664,7 @@
         <v>0</v>
       </c>
       <c r="AF39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG39" t="n">
         <v>0</v>
@@ -5833,36 +4673,6 @@
         <v>0</v>
       </c>
       <c r="AI39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN39" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5940,7 +4750,7 @@
         <v>0</v>
       </c>
       <c r="Y40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z40" t="n">
         <v>0</v>
@@ -5967,39 +4777,9 @@
         <v>0</v>
       </c>
       <c r="AH40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6098,7 +4878,7 @@
         <v>0</v>
       </c>
       <c r="AF41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG41" t="n">
         <v>0</v>
@@ -6107,36 +4887,6 @@
         <v>0</v>
       </c>
       <c r="AI41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN41" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6226,7 +4976,7 @@
         <v>0</v>
       </c>
       <c r="AC42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD42" t="n">
         <v>0</v>
@@ -6244,36 +4994,6 @@
         <v>0</v>
       </c>
       <c r="AI42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK42" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6378,39 +5098,9 @@
         <v>0</v>
       </c>
       <c r="AH43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ43" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6515,39 +5205,9 @@
         <v>0</v>
       </c>
       <c r="AH44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ44" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6652,39 +5312,9 @@
         <v>0</v>
       </c>
       <c r="AH45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6774,7 +5404,7 @@
         <v>0</v>
       </c>
       <c r="AC46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD46" t="n">
         <v>0</v>
@@ -6792,36 +5422,6 @@
         <v>0</v>
       </c>
       <c r="AI46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS46" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6926,39 +5526,9 @@
         <v>0</v>
       </c>
       <c r="AH47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS47" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7063,40 +5633,10 @@
         <v>0</v>
       </c>
       <c r="AH48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI48" t="n">
         <v>0</v>
-      </c>
-      <c r="AJ48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS48" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -7194,7 +5734,7 @@
         <v>0</v>
       </c>
       <c r="AF49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG49" t="n">
         <v>0</v>
@@ -7203,36 +5743,6 @@
         <v>0</v>
       </c>
       <c r="AI49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN49" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS49" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7310,7 +5820,7 @@
         <v>0</v>
       </c>
       <c r="Y50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z50" t="n">
         <v>0</v>
@@ -7319,7 +5829,7 @@
         <v>0</v>
       </c>
       <c r="AB50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC50" t="n">
         <v>0</v>
@@ -7340,36 +5850,6 @@
         <v>0</v>
       </c>
       <c r="AI50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7474,39 +5954,9 @@
         <v>0</v>
       </c>
       <c r="AH51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ51" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS51" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7596,7 +6046,7 @@
         <v>0</v>
       </c>
       <c r="AC52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD52" t="n">
         <v>0</v>
@@ -7614,36 +6064,6 @@
         <v>0</v>
       </c>
       <c r="AI52" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ52" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK52" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL52" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM52" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN52" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO52" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP52" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ52" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR52" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS52" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7742,7 +6162,7 @@
         <v>0</v>
       </c>
       <c r="AF53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG53" t="n">
         <v>0</v>
@@ -7751,36 +6171,6 @@
         <v>0</v>
       </c>
       <c r="AI53" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ53" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK53" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL53" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM53" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN53" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO53" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP53" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ53" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR53" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS53" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7885,39 +6275,9 @@
         <v>0</v>
       </c>
       <c r="AH54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ54" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR54" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS54" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7998,10 +6358,10 @@
         <v>0</v>
       </c>
       <c r="Z55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB55" t="n">
         <v>0</v>
@@ -8025,36 +6385,6 @@
         <v>0</v>
       </c>
       <c r="AI55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR55" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS55" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8150,7 +6480,7 @@
         <v>0</v>
       </c>
       <c r="AE56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF56" t="n">
         <v>0</v>
@@ -8162,36 +6492,6 @@
         <v>0</v>
       </c>
       <c r="AI56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM56" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR56" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8296,39 +6596,9 @@
         <v>0</v>
       </c>
       <c r="AH57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ57" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR57" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS57" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8433,39 +6703,9 @@
         <v>0</v>
       </c>
       <c r="AH58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI58" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ58" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK58" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL58" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM58" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN58" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO58" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP58" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ58" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR58" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS58" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8570,39 +6810,9 @@
         <v>0</v>
       </c>
       <c r="AH59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI59" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ59" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK59" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL59" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM59" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN59" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO59" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP59" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ59" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR59" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS59" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8707,39 +6917,9 @@
         <v>0</v>
       </c>
       <c r="AH60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI60" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ60" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK60" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL60" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM60" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN60" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO60" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP60" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ60" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR60" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS60" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8817,7 +6997,7 @@
         <v>0</v>
       </c>
       <c r="Y61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z61" t="n">
         <v>0</v>
@@ -8826,7 +7006,7 @@
         <v>0</v>
       </c>
       <c r="AB61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC61" t="n">
         <v>0</v>
@@ -8847,36 +7027,6 @@
         <v>0</v>
       </c>
       <c r="AI61" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ61" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK61" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL61" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM61" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN61" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO61" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP61" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ61" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR61" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS61" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8981,39 +7131,9 @@
         <v>0</v>
       </c>
       <c r="AH62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ62" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9118,39 +7238,9 @@
         <v>0</v>
       </c>
       <c r="AH63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI63" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ63" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK63" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL63" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM63" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN63" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO63" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP63" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ63" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR63" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS63" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9249,7 +7339,7 @@
         <v>0</v>
       </c>
       <c r="AF64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG64" t="n">
         <v>0</v>
@@ -9258,36 +7348,6 @@
         <v>0</v>
       </c>
       <c r="AI64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN64" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR64" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS64" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9386,7 +7446,7 @@
         <v>0</v>
       </c>
       <c r="AF65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG65" t="n">
         <v>0</v>
@@ -9395,36 +7455,6 @@
         <v>0</v>
       </c>
       <c r="AI65" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ65" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK65" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL65" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM65" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN65" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO65" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP65" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ65" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR65" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS65" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9502,7 +7532,7 @@
         <v>0</v>
       </c>
       <c r="Y66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z66" t="n">
         <v>0</v>
@@ -9517,7 +7547,7 @@
         <v>0</v>
       </c>
       <c r="AD66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE66" t="n">
         <v>0</v>
@@ -9532,36 +7562,6 @@
         <v>0</v>
       </c>
       <c r="AI66" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ66" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK66" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL66" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM66" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN66" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO66" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP66" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ66" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR66" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS66" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9639,7 +7639,7 @@
         <v>0</v>
       </c>
       <c r="Y67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z67" t="n">
         <v>0</v>
@@ -9654,7 +7654,7 @@
         <v>0</v>
       </c>
       <c r="AD67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE67" t="n">
         <v>0</v>
@@ -9669,36 +7669,6 @@
         <v>0</v>
       </c>
       <c r="AI67" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ67" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK67" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL67" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM67" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN67" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO67" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP67" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ67" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR67" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS67" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9776,7 +7746,7 @@
         <v>0</v>
       </c>
       <c r="Y68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z68" t="n">
         <v>0</v>
@@ -9791,7 +7761,7 @@
         <v>0</v>
       </c>
       <c r="AD68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE68" t="n">
         <v>0</v>
@@ -9806,36 +7776,6 @@
         <v>0</v>
       </c>
       <c r="AI68" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ68" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK68" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL68" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM68" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN68" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO68" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP68" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ68" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR68" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9913,7 +7853,7 @@
         <v>0</v>
       </c>
       <c r="Y69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z69" t="n">
         <v>0</v>
@@ -9928,7 +7868,7 @@
         <v>0</v>
       </c>
       <c r="AD69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE69" t="n">
         <v>0</v>
@@ -9943,36 +7883,6 @@
         <v>0</v>
       </c>
       <c r="AI69" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ69" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK69" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL69" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM69" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN69" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO69" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP69" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ69" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR69" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS69" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10071,7 +7981,7 @@
         <v>0</v>
       </c>
       <c r="AF70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG70" t="n">
         <v>0</v>
@@ -10080,36 +7990,6 @@
         <v>0</v>
       </c>
       <c r="AI70" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ70" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK70" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL70" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM70" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN70" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO70" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP70" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ70" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR70" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS70" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10214,39 +8094,9 @@
         <v>0</v>
       </c>
       <c r="AH71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI71" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ71" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK71" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL71" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM71" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN71" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO71" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP71" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ71" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR71" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS71" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10330,7 +8180,7 @@
         <v>0</v>
       </c>
       <c r="AA72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB72" t="n">
         <v>0</v>
@@ -10342,7 +8192,7 @@
         <v>0</v>
       </c>
       <c r="AE72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF72" t="n">
         <v>0</v>
@@ -10354,36 +8204,6 @@
         <v>0</v>
       </c>
       <c r="AI72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR72" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS72" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10461,7 +8281,7 @@
         <v>0</v>
       </c>
       <c r="Y73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z73" t="n">
         <v>0</v>
@@ -10470,7 +8290,7 @@
         <v>0</v>
       </c>
       <c r="AB73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC73" t="n">
         <v>0</v>
@@ -10491,36 +8311,6 @@
         <v>0</v>
       </c>
       <c r="AI73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR73" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS73" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10625,39 +8415,9 @@
         <v>0</v>
       </c>
       <c r="AH74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI74" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ74" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK74" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL74" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM74" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN74" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO74" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP74" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ74" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR74" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS74" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10735,7 +8495,7 @@
         <v>0</v>
       </c>
       <c r="Y75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z75" t="n">
         <v>0</v>
@@ -10744,7 +8504,7 @@
         <v>0</v>
       </c>
       <c r="AB75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC75" t="n">
         <v>0</v>
@@ -10765,36 +8525,6 @@
         <v>0</v>
       </c>
       <c r="AI75" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ75" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK75" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL75" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM75" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN75" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO75" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP75" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ75" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR75" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10899,39 +8629,9 @@
         <v>0</v>
       </c>
       <c r="AH76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI76" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ76" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK76" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL76" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM76" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN76" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO76" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP76" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ76" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR76" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11021,7 +8721,7 @@
         <v>0</v>
       </c>
       <c r="AC77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD77" t="n">
         <v>0</v>
@@ -11039,36 +8739,6 @@
         <v>0</v>
       </c>
       <c r="AI77" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ77" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK77" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL77" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM77" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN77" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO77" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP77" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ77" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR77" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS77" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11140,10 +8810,10 @@
         <v>0</v>
       </c>
       <c r="W78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y78" t="n">
         <v>0</v>
@@ -11176,36 +8846,6 @@
         <v>0</v>
       </c>
       <c r="AI78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR78" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS78" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11277,10 +8917,10 @@
         <v>1</v>
       </c>
       <c r="W79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y79" t="n">
         <v>0</v>
@@ -11313,36 +8953,6 @@
         <v>0</v>
       </c>
       <c r="AI79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR79" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS79" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11414,10 +9024,10 @@
         <v>0</v>
       </c>
       <c r="W80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y80" t="n">
         <v>0</v>
@@ -11450,36 +9060,6 @@
         <v>0</v>
       </c>
       <c r="AI80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR80" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS80" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11551,10 +9131,10 @@
         <v>0</v>
       </c>
       <c r="W81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y81" t="n">
         <v>0</v>
@@ -11587,36 +9167,6 @@
         <v>0</v>
       </c>
       <c r="AI81" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ81" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK81" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL81" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM81" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN81" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO81" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP81" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ81" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR81" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS81" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11721,39 +9271,9 @@
         <v>0</v>
       </c>
       <c r="AH82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI82" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ82" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK82" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL82" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM82" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN82" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO82" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP82" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ82" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR82" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS82" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11858,39 +9378,9 @@
         <v>0</v>
       </c>
       <c r="AH83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI83" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ83" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK83" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL83" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM83" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN83" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO83" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP83" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ83" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR83" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS83" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11995,39 +9485,9 @@
         <v>0</v>
       </c>
       <c r="AH84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI84" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ84" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK84" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL84" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM84" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN84" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO84" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP84" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ84" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR84" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS84" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12105,10 +9565,10 @@
         <v>0</v>
       </c>
       <c r="Y85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA85" t="n">
         <v>0</v>
@@ -12135,36 +9595,6 @@
         <v>0</v>
       </c>
       <c r="AI85" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ85" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK85" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL85" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM85" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN85" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO85" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP85" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ85" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR85" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12242,10 +9672,10 @@
         <v>0</v>
       </c>
       <c r="Y86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA86" t="n">
         <v>0</v>
@@ -12272,36 +9702,6 @@
         <v>0</v>
       </c>
       <c r="AI86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR86" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS86" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12379,10 +9779,10 @@
         <v>0</v>
       </c>
       <c r="Y87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA87" t="n">
         <v>0</v>
@@ -12409,36 +9809,6 @@
         <v>0</v>
       </c>
       <c r="AI87" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ87" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK87" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL87" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM87" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN87" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO87" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP87" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ87" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR87" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS87" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12525,7 +9895,7 @@
         <v>0</v>
       </c>
       <c r="AB88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC88" t="n">
         <v>0</v>
@@ -12546,36 +9916,6 @@
         <v>0</v>
       </c>
       <c r="AI88" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ88" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK88" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL88" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM88" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN88" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO88" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP88" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ88" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR88" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS88" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12647,10 +9987,10 @@
         <v>0</v>
       </c>
       <c r="W89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y89" t="n">
         <v>0</v>
@@ -12683,36 +10023,6 @@
         <v>0</v>
       </c>
       <c r="AI89" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ89" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK89" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL89" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM89" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN89" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO89" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP89" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ89" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR89" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS89" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12796,7 +10106,7 @@
         <v>0</v>
       </c>
       <c r="AA90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB90" t="n">
         <v>0</v>
@@ -12820,36 +10130,6 @@
         <v>0</v>
       </c>
       <c r="AI90" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR90" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS90" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12951,42 +10231,12 @@
         <v>0</v>
       </c>
       <c r="AG91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH91" t="n">
         <v>0</v>
       </c>
       <c r="AI91" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ91" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK91" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL91" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM91" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN91" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO91" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP91" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ91" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR91" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS91" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13076,7 +10326,7 @@
         <v>0</v>
       </c>
       <c r="AC92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD92" t="n">
         <v>0</v>
@@ -13094,36 +10344,6 @@
         <v>0</v>
       </c>
       <c r="AI92" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ92" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK92" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL92" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM92" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN92" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO92" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP92" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ92" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR92" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS92" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13228,39 +10448,9 @@
         <v>0</v>
       </c>
       <c r="AH93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI93" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ93" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK93" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL93" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM93" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN93" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO93" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP93" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ93" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR93" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS93" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13338,7 +10528,7 @@
         <v>0</v>
       </c>
       <c r="Y94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z94" t="n">
         <v>0</v>
@@ -13347,7 +10537,7 @@
         <v>0</v>
       </c>
       <c r="AB94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC94" t="n">
         <v>0</v>
@@ -13368,36 +10558,6 @@
         <v>0</v>
       </c>
       <c r="AI94" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ94" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK94" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL94" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM94" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN94" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO94" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP94" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ94" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR94" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS94" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13475,7 +10635,7 @@
         <v>0</v>
       </c>
       <c r="Y95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z95" t="n">
         <v>0</v>
@@ -13484,7 +10644,7 @@
         <v>0</v>
       </c>
       <c r="AB95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC95" t="n">
         <v>0</v>
@@ -13505,36 +10665,6 @@
         <v>0</v>
       </c>
       <c r="AI95" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ95" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK95" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL95" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM95" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN95" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO95" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP95" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ95" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR95" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS95" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13639,39 +10769,9 @@
         <v>0</v>
       </c>
       <c r="AH96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ96" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR96" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS96" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13743,10 +10843,10 @@
         <v>0</v>
       </c>
       <c r="W97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y97" t="n">
         <v>0</v>
@@ -13779,36 +10879,6 @@
         <v>0</v>
       </c>
       <c r="AI97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR97" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS97" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13886,7 +10956,7 @@
         <v>0</v>
       </c>
       <c r="Y98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z98" t="n">
         <v>0</v>
@@ -13895,7 +10965,7 @@
         <v>0</v>
       </c>
       <c r="AB98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC98" t="n">
         <v>0</v>
@@ -13916,36 +10986,6 @@
         <v>0</v>
       </c>
       <c r="AI98" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ98" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK98" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL98" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM98" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN98" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO98" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP98" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ98" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR98" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS98" t="n">
         <v>0</v>
       </c>
     </row>
@@ -14029,13 +11069,13 @@
         <v>0</v>
       </c>
       <c r="AA99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB99" t="n">
         <v>0</v>
       </c>
       <c r="AC99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD99" t="n">
         <v>0</v>
@@ -14053,36 +11093,6 @@
         <v>0</v>
       </c>
       <c r="AI99" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ99" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK99" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL99" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM99" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN99" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO99" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP99" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ99" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR99" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS99" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>